<commit_message>
adding inv feed  sold seats code
</commit_message>
<xml_diff>
--- a/mvc/downloads/invfeed.xlsx
+++ b/mvc/downloads/invfeed.xlsx
@@ -1,14 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21830"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_fcf\AC\Temp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9BB5282C-BC3C-48E6-AD44-C00955A0DC24}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{ED5312D7-1494-415D-886A-185F3C1ED73E}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="19">
   <si>
     <t>Airlline code</t>
   </si>
@@ -39,6 +34,9 @@
     <t>Dept date</t>
   </si>
   <si>
+    <t>Origin Airport</t>
+  </si>
+  <si>
     <t>Destination Airport</t>
   </si>
   <si>
@@ -48,59 +46,47 @@
     <t>Empty seats</t>
   </si>
   <si>
-    <t>Sold seats</t>
-  </si>
-  <si>
     <t>SQ</t>
   </si>
   <si>
     <t>SQ1234</t>
   </si>
   <si>
+    <t>KUL</t>
+  </si>
+  <si>
+    <t>COK</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>SQ1235</t>
+  </si>
+  <si>
     <t>SIN</t>
   </si>
   <si>
     <t>SFO</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>SQ1235</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
     <t>SQ1236</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>SQ1237</t>
-  </si>
-  <si>
-    <t>SQ1238</t>
-  </si>
-  <si>
-    <t>SQ1239</t>
-  </si>
-  <si>
-    <t>SQ1240</t>
-  </si>
-  <si>
-    <t>SQ1241</t>
-  </si>
-  <si>
-    <t>Origin Airport</t>
+    <t>HND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,18 +432,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,22 +454,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -491,7 +474,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>43536</v>
+        <v>43639</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -505,19 +488,16 @@
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>43537</v>
+        <v>43639</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -526,24 +506,21 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>23</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>43538</v>
+        <v>43639</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -552,16 +529,13 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>22</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -569,13 +543,13 @@
         <v>14</v>
       </c>
       <c r="C5" s="1">
-        <v>43539</v>
+        <v>43639</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -583,77 +557,68 @@
       <c r="G5">
         <v>34</v>
       </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43639</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1">
-        <v>43540</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>33</v>
       </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
-        <v>43541</v>
+        <v>43639</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7">
         <v>45</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43639</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1">
-        <v>43542</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -661,60 +626,51 @@
       <c r="G8">
         <v>33</v>
       </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
-        <v>43543</v>
+        <v>43639</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9">
         <v>12</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
-        <v>43544</v>
+        <v>43639</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G10">
         <v>11</v>
-      </c>
-      <c r="H10">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>